<commit_message>
Project HLR and Defect Report
Project HLR and Defect Report
</commit_message>
<xml_diff>
--- a/Project HLR.xlsx
+++ b/Project HLR.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\upadh\Desktop\TOPS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\upadh\Desktop\TOPS\Project Demo Blaze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{827ADF3A-03F7-4E46-AB06-089D32AF0C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E161C45-0D10-4949-BD4D-B97452CFD7B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F59B7418-4575-41AE-9947-61218B685AF8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{F59B7418-4575-41AE-9947-61218B685AF8}"/>
   </bookViews>
   <sheets>
     <sheet name="HLR Demo Blaze Project" sheetId="1" r:id="rId1"/>
+    <sheet name="Defect Report" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="143">
   <si>
     <t>HLR Of Demo Blaze</t>
   </si>
@@ -288,13 +289,210 @@
   </si>
   <si>
     <t>Check for texts written in footer,it should be readeble,correct spellings etc.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Internet, working wbsite, browser</t>
+  </si>
+  <si>
+    <t>Test case name</t>
+  </si>
+  <si>
+    <t>Test case ID</t>
+  </si>
+  <si>
+    <t>Pre-condition</t>
+  </si>
+  <si>
+    <t>Test step</t>
+  </si>
+  <si>
+    <t>Test data</t>
+  </si>
+  <si>
+    <t>Expected Outcome</t>
+  </si>
+  <si>
+    <t>Actual Outcome</t>
+  </si>
+  <si>
+    <t>Test Case Demo Blaze</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>1.Open url: https://www.demoblaze.com/ 2.Click on slide button</t>
+  </si>
+  <si>
+    <t>1.Open url: https://www.demoblaze.com/ 2.Click on categories button</t>
+  </si>
+  <si>
+    <t>1.Open url: https://www.demoblaze.com/ 2.Click on phone button</t>
+  </si>
+  <si>
+    <t>1.Open url: https://www.demoblaze.com/ 2.Click on laptop button</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>It only shows two categories picture not monitor categories picture.</t>
+  </si>
+  <si>
+    <t>Shows different categories picture .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shows different categories picture and its description. </t>
+  </si>
+  <si>
+    <t>Shows different phone picture and its description.</t>
+  </si>
+  <si>
+    <t>Shows different laptop picture and its description.</t>
+  </si>
+  <si>
+    <t>Its shows same picture with different categories description.</t>
+  </si>
+  <si>
+    <t>Its shows same picture with different laptop description.</t>
+  </si>
+  <si>
+    <t>Its shows same picture with different phone description.</t>
+  </si>
+  <si>
+    <t>1.Enter the URL  http://www.demoblaze.com 
+2. Click on the contact button
+3.Enter valid data
+4.click on send message button</t>
+  </si>
+  <si>
+    <t>1.Enter the URL  http://www.demoblaze.com 
+2. Click on the contact button
+3.Dont enter any data
+4.click on send message button</t>
+  </si>
+  <si>
+    <t>1.Enter the URL  http://www.demoblaze.com 
+2. Click on the contact button
+3.Dont write any message
+4.click on send message button</t>
+  </si>
+  <si>
+    <t>The message should not get sent</t>
+  </si>
+  <si>
+    <t>Not as per desined</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The message is getting sent </t>
+  </si>
+  <si>
+    <t>Check the demoblaze brand name button</t>
+  </si>
+  <si>
+    <t>1.Open url: https://www.demoblaze.com/ 2.Click on monitor button</t>
+  </si>
+  <si>
+    <t>Shows different monitor picture and its description.</t>
+  </si>
+  <si>
+    <t>Shows different categories picture.</t>
+  </si>
+  <si>
+    <t>Shows same product image.</t>
+  </si>
+  <si>
+    <t>Image is not correct</t>
+  </si>
+  <si>
+    <t>Defect ID</t>
+  </si>
+  <si>
+    <t>Defect type</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Severity</t>
+  </si>
+  <si>
+    <t>Screenshots/Video</t>
+  </si>
+  <si>
+    <t>Contact email:p@gmail
+Contact name: p123</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The brand name should be as per the requirement</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1QuevhL9xYMhw6h-ow9y8ai6fIKd0sBjE/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Lp5C1FxayRAQ3-xeUhI-SgUTFByWScl3/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1qbuuFqtfFfo03BBi8i1FiUGgA9AV6m3R/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1RS-GYN6N053nPMojWCvhB8f94IDzJN29/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Ox5T4mXDA-AcSAlaxjB3pjgPPDD7fOJv/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1uxxGH4Io4G3GizQcrPBQkg0GfZM0s0UU/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1qkPgwe5LJXjxCFDYfZaaKUOOViUy6b1s/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1QgdywtyjihSoZWXta5g2bT0qqRD5l8Ec/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1Y91avpbM2IyYqDgaCskTd4-m93_yTfP6/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Functanality Defect</t>
+  </si>
+  <si>
+    <t>1.Enter the URL  http://www.demoblaze.com 
+2. Click product to add to cart 3. Click on place order button 4.Fill up detail wrong</t>
+  </si>
+  <si>
+    <t>Product is purched message successfully</t>
+  </si>
+  <si>
+    <t>Invalid data</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1n-t3aX56LH45sh14t5FJ3wXyxbFvD7_9/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1S8JkuKLl_vvLF3yheY8fTvWAGVJy-PFS/view?usp=share_link</t>
+  </si>
+  <si>
+    <t>Name: Parth,Country : India,City:Surat,Credit Card : 123456780,Month: 10,Year: 2024</t>
+  </si>
+  <si>
+    <t>Name: Parth,Country : India,City:Surat,Credit Card : 123456,Month: 10,Year: 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,32 +523,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -361,19 +588,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -394,11 +608,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -421,39 +670,469 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -486,6 +1165,26 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -531,12 +1230,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5B40A08-6F1E-4B66-A2CA-BD60517C4FBA}" name="Table6910" displayName="Table6910" ref="C7:E49" totalsRowShown="0" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A5B40A08-6F1E-4B66-A2CA-BD60517C4FBA}" name="Table6910" displayName="Table6910" ref="C7:E49" totalsRowShown="0" dataDxfId="17">
   <autoFilter ref="C7:E49" xr:uid="{AC7E6479-5091-4CB4-9CDC-C1BD49D70EDB}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{509D36C4-4C8D-4BEF-A6C1-3DC7753FD7ED}" name="Functionality ID" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{D9E04DD7-71F2-4001-B6F4-D769A018AD22}" name="Functionality Name" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{C8E4DACE-EF5E-4863-A6EC-1145A2588361}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{509D36C4-4C8D-4BEF-A6C1-3DC7753FD7ED}" name="Functionality ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{D9E04DD7-71F2-4001-B6F4-D769A018AD22}" name="Functionality Name" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{C8E4DACE-EF5E-4863-A6EC-1145A2588361}" name="Description" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6C2C031F-5B4F-4988-AECA-B950DB22AE32}" name="Table691035" displayName="Table691035" ref="C7:N19" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="C7:N19" xr:uid="{AC7E6479-5091-4CB4-9CDC-C1BD49D70EDB}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{815E6B46-3BA4-445C-9E03-390501AFE6C3}" name="Functionality ID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{1A62F1A8-70F1-4C32-9D36-2DA72377A07E}" name="Test case name" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{C6FF6D26-D700-49DC-B5FA-7D2A323EFCD1}" name="Pre-condition" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{232F7ACD-79EB-40AF-8D3E-226B7DA6A0AA}" name="Test step" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{DC7FB56C-4DFF-4C08-A3D5-FAA13DD86576}" name="Test data" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{DE9BBFEB-5322-4BF7-9FC4-92C0FDC360F9}" name="Defect type" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{8B64EE9A-D67F-4266-B6ED-CBD710F4C3C6}" name="Severity" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{59263DE2-22BD-4077-9280-7EDA5998560B}" name="Priority" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{0D63B96B-BDB8-497B-9F71-52A2578E61DF}" name="Expected Outcome" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{5084B6B8-5646-4CAC-820C-C4DD08109E3B}" name="Actual Outcome" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{0C0EFA41-1649-4D0C-A40A-70E39085AD35}" name="Screenshots/Video" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{0304521A-EF89-44DC-A7A9-6E117459FE1A}" name="Status" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -841,14 +1561,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E340FE4-25C7-47E8-95EB-32C16F3C2B0D}">
   <dimension ref="C2:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="19.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5546875" style="17" customWidth="1"/>
+    <col min="4" max="4" width="39.5546875" style="13" customWidth="1"/>
     <col min="5" max="5" width="127.44140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
@@ -873,10 +1593,10 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -884,10 +1604,10 @@
       <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>7</v>
       </c>
     </row>
@@ -895,10 +1615,10 @@
       <c r="C10" s="1">
         <v>3</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -906,10 +1626,10 @@
       <c r="C11" s="1">
         <v>4</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>11</v>
       </c>
     </row>
@@ -917,10 +1637,10 @@
       <c r="C12" s="1">
         <v>5</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>13</v>
       </c>
     </row>
@@ -928,10 +1648,10 @@
       <c r="C13" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -939,10 +1659,10 @@
       <c r="C14" s="1">
         <v>5.2</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -950,10 +1670,10 @@
       <c r="C15" s="1">
         <v>6</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -961,10 +1681,10 @@
       <c r="C16" s="1">
         <v>6.1</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -972,10 +1692,10 @@
       <c r="C17" s="1">
         <v>6.2</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="8" t="s">
         <v>22</v>
       </c>
     </row>
@@ -983,10 +1703,10 @@
       <c r="C18" s="1">
         <v>6.3</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
@@ -994,10 +1714,10 @@
       <c r="C19" s="1">
         <v>6.4</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1005,10 +1725,10 @@
       <c r="C20" s="1">
         <v>6.5</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="8" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1016,10 +1736,10 @@
       <c r="C21" s="1">
         <v>6.6</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1027,21 +1747,21 @@
       <c r="C22" s="1">
         <v>6.7</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="3:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="C23" s="12">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23" s="9">
         <v>6.8</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="8" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1049,21 +1769,21 @@
       <c r="C24" s="1">
         <v>6.9</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="3:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="C25" s="12" t="s">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="8" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1071,10 +1791,10 @@
       <c r="C26" s="1">
         <v>6.11</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1082,10 +1802,10 @@
       <c r="C27" s="1">
         <v>7</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="7" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1093,10 +1813,10 @@
       <c r="C28" s="1">
         <v>7.1</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="7" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1104,10 +1824,10 @@
       <c r="C29" s="1">
         <v>7.2</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="E29" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1115,10 +1835,10 @@
       <c r="C30" s="1">
         <v>7.3</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="E30" s="7" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1126,10 +1846,10 @@
       <c r="C31" s="1">
         <v>7.4</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="7" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1137,10 +1857,10 @@
       <c r="C32" s="1">
         <v>8</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1148,10 +1868,10 @@
       <c r="C33" s="1">
         <v>8.1</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1159,10 +1879,10 @@
       <c r="C34" s="1">
         <v>8.1999999999999993</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1170,10 +1890,10 @@
       <c r="C35" s="1">
         <v>9</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="7" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1181,10 +1901,10 @@
       <c r="C36" s="1">
         <v>10</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="7" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1192,10 +1912,10 @@
       <c r="C37" s="1">
         <v>10.1</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="7" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1203,10 +1923,10 @@
       <c r="C38" s="1">
         <v>10.199999999999999</v>
       </c>
-      <c r="D38" s="8" t="s">
+      <c r="D38" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1214,10 +1934,10 @@
       <c r="C39" s="1">
         <v>11</v>
       </c>
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="14" t="s">
+      <c r="E39" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1225,10 +1945,10 @@
       <c r="C40" s="1">
         <v>12</v>
       </c>
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="7" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1236,10 +1956,10 @@
       <c r="C41" s="1">
         <v>13</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="D41" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1247,10 +1967,10 @@
       <c r="C42" s="1">
         <v>14</v>
       </c>
-      <c r="D42" s="8" t="s">
+      <c r="D42" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1258,10 +1978,10 @@
       <c r="C43" s="1">
         <v>15</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="7" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1269,21 +1989,21 @@
       <c r="C44" s="1">
         <v>16</v>
       </c>
-      <c r="D44" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="45" spans="3:5" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="C45" s="12">
+      <c r="C45" s="9">
         <v>17</v>
       </c>
-      <c r="D45" s="10" t="s">
+      <c r="D45" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="11" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1291,10 +2011,10 @@
       <c r="C46" s="1">
         <v>17.100000000000001</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="7" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1302,10 +2022,10 @@
       <c r="C47" s="1">
         <v>18</v>
       </c>
-      <c r="D47" s="8" t="s">
+      <c r="D47" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1313,10 +2033,10 @@
       <c r="C48" s="1">
         <v>19</v>
       </c>
-      <c r="D48" s="8" t="s">
+      <c r="D48" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="7" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1324,10 +2044,10 @@
       <c r="C49" s="1">
         <v>20</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="E49" s="12" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1338,4 +2058,617 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382E3D1E-6169-440A-BE8F-BDC8B526CD83}">
+  <dimension ref="A2:N19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" style="13" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" customWidth="1"/>
+    <col min="13" max="13" width="14.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="D2" s="2"/>
+      <c r="G2" s="27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="M7" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="N7" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="21">
+        <v>1</v>
+      </c>
+      <c r="B8" s="21">
+        <v>9</v>
+      </c>
+      <c r="C8" s="21">
+        <v>3</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H8" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="N8" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="21">
+        <v>2</v>
+      </c>
+      <c r="B9" s="21">
+        <v>20</v>
+      </c>
+      <c r="C9" s="21">
+        <v>5</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="M9" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="N9" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="21">
+        <v>3</v>
+      </c>
+      <c r="B10" s="21">
+        <v>22</v>
+      </c>
+      <c r="C10" s="21">
+        <v>5</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="L10" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="M10" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="N10" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="21">
+        <v>4</v>
+      </c>
+      <c r="B11" s="21">
+        <v>23</v>
+      </c>
+      <c r="C11" s="21">
+        <v>5</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="L11" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="M11" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
+        <v>5</v>
+      </c>
+      <c r="B12" s="21">
+        <v>27</v>
+      </c>
+      <c r="C12" s="21">
+        <v>12</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="L12" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="M12" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="N12" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="21">
+        <v>6</v>
+      </c>
+      <c r="B13" s="21">
+        <v>28</v>
+      </c>
+      <c r="C13" s="21">
+        <v>13</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K13" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="L13" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="M13" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="N13" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="21">
+        <v>7</v>
+      </c>
+      <c r="B14" s="21">
+        <v>29</v>
+      </c>
+      <c r="C14" s="21">
+        <v>14</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="L14" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="M14" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="N14" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="21">
+        <v>8</v>
+      </c>
+      <c r="B15" s="21">
+        <v>30</v>
+      </c>
+      <c r="C15" s="21">
+        <v>15</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="L15" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="M15" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="N15" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="22">
+        <v>9</v>
+      </c>
+      <c r="B16" s="22">
+        <v>31</v>
+      </c>
+      <c r="C16" s="23">
+        <v>16</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I16" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K16" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="L16" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="M16" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="N16" s="24" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="124.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="22">
+        <v>10</v>
+      </c>
+      <c r="B17" s="22">
+        <v>32</v>
+      </c>
+      <c r="C17" s="21">
+        <v>17</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H17" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="L17" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="N17" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="29">
+        <v>11</v>
+      </c>
+      <c r="B18" s="22">
+        <v>52</v>
+      </c>
+      <c r="C18" s="28">
+        <v>7.3</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="L18" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="M18" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="156" x14ac:dyDescent="0.3">
+      <c r="A19" s="22">
+        <v>12</v>
+      </c>
+      <c r="B19" s="22">
+        <v>52</v>
+      </c>
+      <c r="C19" s="28">
+        <v>7.3</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="J19" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="K19" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="L19" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="M19" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>